<commit_message>
parts of inventory based on specifications
</commit_message>
<xml_diff>
--- a/Arad.Portal.UI.Shop/wwwroot/Dictionaries/DictionaryTemplate.xlsx
+++ b/Arad.Portal.UI.Shop/wwwroot/Dictionaries/DictionaryTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AradProject\arad.portal\Arad.Portal.UI.Shop\wwwroot\Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598AB6DA-63EB-4D98-9315-F80D98A3EE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37E2470-18B1-4074-9C01-041A958FCD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="764">
   <si>
     <t>Key</t>
   </si>
@@ -2302,6 +2302,21 @@
   </si>
   <si>
     <t>AlertAndMessage_EmailInvalid</t>
+  </si>
+  <si>
+    <t>AlertAndMessage_UserNotFound</t>
+  </si>
+  <si>
+    <t>AlertAndMessage_ChangePassConfirmation</t>
+  </si>
+  <si>
+    <t>btn_Close</t>
+  </si>
+  <si>
+    <t>btn_Copy</t>
+  </si>
+  <si>
+    <t>AlertAndMessage_CopyDone</t>
   </si>
 </sst>
 </file>
@@ -2628,10 +2643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C757"/>
+  <dimension ref="A1:C762"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A745" workbookViewId="0">
-      <selection activeCell="A757" sqref="A757"/>
+      <selection activeCell="A762" sqref="A762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6432,6 +6447,31 @@
         <v>758</v>
       </c>
     </row>
+    <row r="758" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A758" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="759" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A759" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="760" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A760" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="761" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A761" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="762" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A762" t="s">
+        <v>763</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
shipping and specification inventory check
</commit_message>
<xml_diff>
--- a/Arad.Portal.UI.Shop/wwwroot/Dictionaries/DictionaryTemplate.xlsx
+++ b/Arad.Portal.UI.Shop/wwwroot/Dictionaries/DictionaryTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AradProject\arad.portal\Arad.Portal.UI.Shop\wwwroot\Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39686814-48B2-4059-84A9-BD6AA0F27A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3460BD-191D-4D3B-A30C-2D560A9BE683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="767">
   <si>
     <t>Key</t>
   </si>
@@ -2323,6 +2323,9 @@
   </si>
   <si>
     <t>AlertAndMessage_FillSpecValues</t>
+  </si>
+  <si>
+    <t>AlertAndMessage_UpdateProductInventory</t>
   </si>
 </sst>
 </file>
@@ -2649,10 +2652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C764"/>
+  <dimension ref="A1:C765"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A745" workbookViewId="0">
-      <selection activeCell="A764" sqref="A764"/>
+      <selection activeCell="A765" sqref="A765"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6488,6 +6491,11 @@
         <v>765</v>
       </c>
     </row>
+    <row r="765" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A765" t="s">
+        <v>766</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
install and redirect parts
</commit_message>
<xml_diff>
--- a/Arad.Portal.UI.Shop/wwwroot/Dictionaries/DictionaryTemplate.xlsx
+++ b/Arad.Portal.UI.Shop/wwwroot/Dictionaries/DictionaryTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AradProject\Arad.Portal\Arad.Portal.UI.Shop\wwwroot\Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6E6231-9305-42D1-8154-8AC66314C312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD7A497-D4A9-44B1-B8DB-0715F55FC316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="780">
   <si>
     <t>Key</t>
   </si>
@@ -2350,6 +2350,21 @@
   </si>
   <si>
     <t>Discount</t>
+  </si>
+  <si>
+    <t>DomainSMTPAcc</t>
+  </si>
+  <si>
+    <t>SMTPServer</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
+  </si>
+  <si>
+    <t>ServerPort</t>
+  </si>
+  <si>
+    <t>EncryptionType</t>
   </si>
 </sst>
 </file>
@@ -2676,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C773"/>
+  <dimension ref="A1:C778"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A769" workbookViewId="0">
-      <selection activeCell="A773" sqref="A773"/>
+      <selection activeCell="A778" sqref="A778"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6560,6 +6575,31 @@
         <v>774</v>
       </c>
     </row>
+    <row r="774" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="775" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A775" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="776" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A776" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="777" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A777" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A778" t="s">
+        <v>779</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>